<commit_message>
fixed test vector expected values
</commit_message>
<xml_diff>
--- a/TestProgram.xlsx
+++ b/TestProgram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cnorf\Documents\GitHub\vlsi-2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC6BE43-26FF-4D27-8FAC-A33C0A5B243A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B090C973-7170-4F78-8444-9C21B8CB8BCA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FAE62355-45BA-4BDC-BDE4-E66D9B9007D9}"/>
   </bookViews>
@@ -162,9 +162,6 @@
     <t>storer R4, R7</t>
   </si>
   <si>
-    <t>Test succeedes if 64 written in addr 65</t>
-  </si>
-  <si>
     <t>Addr</t>
   </si>
   <si>
@@ -177,19 +174,22 @@
     <t>Program Memory</t>
   </si>
   <si>
-    <t>64, 0</t>
-  </si>
-  <si>
     <t>set before test</t>
   </si>
   <si>
-    <t>64 if test passes, 0 if test fails</t>
-  </si>
-  <si>
     <t>setn R7, 41</t>
   </si>
   <si>
     <t>setn R0, 40</t>
+  </si>
+  <si>
+    <t>45, 0</t>
+  </si>
+  <si>
+    <t>Test succeedes if 45 written in addr 65</t>
+  </si>
+  <si>
+    <t>45 if test passes, 0 if test fails</t>
   </si>
 </sst>
 </file>
@@ -589,7 +589,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -599,7 +599,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -653,10 +653,10 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C4">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -688,7 +688,7 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -724,7 +724,7 @@
         <v>14</v>
       </c>
       <c r="C6">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -757,7 +757,7 @@
         <v>15</v>
       </c>
       <c r="C7">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -790,7 +790,7 @@
         <v>16</v>
       </c>
       <c r="C8">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -799,7 +799,8 @@
         <v>-5</v>
       </c>
       <c r="F8">
-        <v>59</v>
+        <f>C8+E8</f>
+        <v>35</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -823,7 +824,7 @@
         <v>19</v>
       </c>
       <c r="C9">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -832,10 +833,12 @@
         <v>-5</v>
       </c>
       <c r="F9">
-        <v>59</v>
+        <f t="shared" ref="F9:F35" si="1">C9+E9</f>
+        <v>35</v>
       </c>
       <c r="G9">
-        <v>64</v>
+        <f>C9-E9</f>
+        <v>45</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -856,7 +859,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="1">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D10" s="1">
         <v>5</v>
@@ -865,10 +868,12 @@
         <v>-5</v>
       </c>
       <c r="F10" s="1">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G10" s="1">
-        <v>64</v>
+        <f>C10-E10</f>
+        <v>45</v>
       </c>
       <c r="H10" s="1">
         <v>0</v>
@@ -892,7 +897,7 @@
         <v>23</v>
       </c>
       <c r="C11" s="1">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1">
         <v>5</v>
@@ -901,7 +906,8 @@
         <v>-5</v>
       </c>
       <c r="F11" s="1">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
@@ -928,7 +934,7 @@
         <v>26</v>
       </c>
       <c r="C12" s="2">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D12" s="2">
         <v>5</v>
@@ -937,10 +943,11 @@
         <v>-5</v>
       </c>
       <c r="F12" s="2">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G12" s="2">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="H12" s="2">
         <v>11</v>
@@ -961,7 +968,7 @@
         <v>28</v>
       </c>
       <c r="C13" s="2">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D13" s="2">
         <v>5</v>
@@ -970,10 +977,11 @@
         <v>-5</v>
       </c>
       <c r="F13" s="2">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G13" s="2">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="H13" s="2">
         <v>11</v>
@@ -997,7 +1005,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="2">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D14" s="2">
         <v>5</v>
@@ -1006,7 +1014,8 @@
         <v>-5</v>
       </c>
       <c r="F14" s="2">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G14" s="2">
         <v>0</v>
@@ -1030,7 +1039,7 @@
         <v>29</v>
       </c>
       <c r="C15" s="3">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D15" s="3">
         <v>5</v>
@@ -1039,10 +1048,11 @@
         <v>-5</v>
       </c>
       <c r="F15" s="3">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G15" s="3">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="H15" s="3">
         <v>11</v>
@@ -1066,7 +1076,7 @@
         <v>23</v>
       </c>
       <c r="C16" s="3">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D16" s="3">
         <v>5</v>
@@ -1075,7 +1085,8 @@
         <v>-5</v>
       </c>
       <c r="F16" s="3">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G16" s="3">
         <v>0</v>
@@ -1099,7 +1110,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="3">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D17" s="3">
         <v>5</v>
@@ -1108,10 +1119,11 @@
         <v>-5</v>
       </c>
       <c r="F17" s="3">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G17" s="3">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="H17" s="3">
         <v>11</v>
@@ -1135,7 +1147,7 @@
         <v>35</v>
       </c>
       <c r="C18" s="3">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D18" s="3">
         <v>5</v>
@@ -1144,10 +1156,11 @@
         <v>-5</v>
       </c>
       <c r="F18" s="3">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G18" s="3">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="H18" s="3">
         <v>11</v>
@@ -1171,7 +1184,7 @@
         <v>30</v>
       </c>
       <c r="C19" s="4">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D19" s="4">
         <v>5</v>
@@ -1180,10 +1193,11 @@
         <v>-5</v>
       </c>
       <c r="F19" s="4">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G19" s="4">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="H19" s="4">
         <v>11</v>
@@ -1207,7 +1221,7 @@
         <v>23</v>
       </c>
       <c r="C20" s="4">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D20" s="4">
         <v>5</v>
@@ -1216,7 +1230,8 @@
         <v>-5</v>
       </c>
       <c r="F20" s="4">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G20" s="4">
         <v>0</v>
@@ -1240,7 +1255,7 @@
         <v>31</v>
       </c>
       <c r="C21" s="4">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D21" s="4">
         <v>5</v>
@@ -1249,10 +1264,11 @@
         <v>-5</v>
       </c>
       <c r="F21" s="4">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G21" s="4">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="H21" s="4">
         <v>11</v>
@@ -1276,7 +1292,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="4">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D22" s="4">
         <v>5</v>
@@ -1285,7 +1301,8 @@
         <v>-5</v>
       </c>
       <c r="F22" s="4">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G22" s="4">
         <v>0</v>
@@ -1309,7 +1326,7 @@
         <v>36</v>
       </c>
       <c r="C23" s="4">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D23" s="4">
         <v>5</v>
@@ -1318,10 +1335,11 @@
         <v>-5</v>
       </c>
       <c r="F23" s="4">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G23" s="4">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="H23" s="4">
         <v>11</v>
@@ -1345,7 +1363,7 @@
         <v>32</v>
       </c>
       <c r="C24" s="5">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D24" s="5">
         <v>5</v>
@@ -1354,10 +1372,11 @@
         <v>-5</v>
       </c>
       <c r="F24" s="5">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G24" s="5">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="H24" s="5">
         <v>11</v>
@@ -1381,7 +1400,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="5">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D25" s="5">
         <v>5</v>
@@ -1390,7 +1409,8 @@
         <v>-5</v>
       </c>
       <c r="F25" s="5">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G25" s="5">
         <v>0</v>
@@ -1413,7 +1433,7 @@
         <v>37</v>
       </c>
       <c r="C26" s="5">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D26" s="5">
         <v>5</v>
@@ -1422,10 +1442,11 @@
         <v>-5</v>
       </c>
       <c r="F26" s="5">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G26" s="5">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="H26" s="5">
         <v>11</v>
@@ -1448,7 +1469,7 @@
         <v>38</v>
       </c>
       <c r="C27" s="5">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D27" s="5">
         <v>5</v>
@@ -1457,10 +1478,11 @@
         <v>-5</v>
       </c>
       <c r="F27" s="5">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G27" s="5">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="H27" s="5">
         <v>11</v>
@@ -1483,7 +1505,7 @@
         <v>33</v>
       </c>
       <c r="C28" s="6">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D28" s="6">
         <v>5</v>
@@ -1492,10 +1514,11 @@
         <v>-5</v>
       </c>
       <c r="F28" s="6">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G28" s="6">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="H28" s="6">
         <v>11</v>
@@ -1518,7 +1541,7 @@
         <v>23</v>
       </c>
       <c r="C29" s="6">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D29" s="6">
         <v>5</v>
@@ -1527,7 +1550,8 @@
         <v>-5</v>
       </c>
       <c r="F29" s="6">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G29" s="6">
         <v>0</v>
@@ -1550,7 +1574,7 @@
         <v>39</v>
       </c>
       <c r="C30" s="6">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D30" s="6">
         <v>5</v>
@@ -1559,10 +1583,11 @@
         <v>-5</v>
       </c>
       <c r="F30" s="6">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G30" s="6">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="H30" s="6">
         <v>11</v>
@@ -1585,7 +1610,7 @@
         <v>40</v>
       </c>
       <c r="C31" s="6">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D31" s="6">
         <v>5</v>
@@ -1594,10 +1619,11 @@
         <v>-5</v>
       </c>
       <c r="F31" s="6">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G31" s="6">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="H31" s="6">
         <v>11</v>
@@ -1621,7 +1647,7 @@
         <v>41</v>
       </c>
       <c r="C32">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D32">
         <v>5</v>
@@ -1630,10 +1656,11 @@
         <v>-5</v>
       </c>
       <c r="F32">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G32">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="H32">
         <v>11</v>
@@ -1654,7 +1681,7 @@
         <v>23</v>
       </c>
       <c r="C33">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D33">
         <v>5</v>
@@ -1663,10 +1690,11 @@
         <v>-5</v>
       </c>
       <c r="F33">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G33">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="H33">
         <v>11</v>
@@ -1687,10 +1715,10 @@
         <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C34">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D34">
         <v>5</v>
@@ -1699,10 +1727,11 @@
         <v>-5</v>
       </c>
       <c r="F34">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G34">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="H34">
         <v>11</v>
@@ -1723,7 +1752,7 @@
         <v>42</v>
       </c>
       <c r="C35">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D35">
         <v>5</v>
@@ -1732,10 +1761,11 @@
         <v>-5</v>
       </c>
       <c r="F35">
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="G35">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="H35">
         <v>11</v>
@@ -1747,20 +1777,20 @@
         <v>41</v>
       </c>
       <c r="M35" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
@@ -1771,7 +1801,7 @@
         <v>5</v>
       </c>
       <c r="L38" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
@@ -1779,10 +1809,10 @@
         <v>41</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L39" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed test program to deal with x in rf at init
</commit_message>
<xml_diff>
--- a/TestProgram.xlsx
+++ b/TestProgram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cnorf\Documents\GitHub\vlsi-2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B090C973-7170-4F78-8444-9C21B8CB8BCA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B40DF46-6B6F-4D5D-AE3F-29C30A02E089}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FAE62355-45BA-4BDC-BDE4-E66D9B9007D9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="55">
   <si>
     <t>Instruction</t>
   </si>
@@ -120,45 +120,6 @@
     <t>jumpr R5</t>
   </si>
   <si>
-    <t>jeqzn R6, 13</t>
-  </si>
-  <si>
-    <t>jnezn R1, 17</t>
-  </si>
-  <si>
-    <t>jnezn R2, 19</t>
-  </si>
-  <si>
-    <t>jgtzn R1, 22</t>
-  </si>
-  <si>
-    <t>jltzn R2, 26</t>
-  </si>
-  <si>
-    <t>jeqzn R1, 29</t>
-  </si>
-  <si>
-    <t>jeqzn R2, 29</t>
-  </si>
-  <si>
-    <t>jnezn R2, 29</t>
-  </si>
-  <si>
-    <t>jgtzn R2, 29</t>
-  </si>
-  <si>
-    <t>jgtzn R6, 29</t>
-  </si>
-  <si>
-    <t>jltzn R1, 29</t>
-  </si>
-  <si>
-    <t>jltzn R6, 29</t>
-  </si>
-  <si>
-    <t>jumpn 30</t>
-  </si>
-  <si>
     <t>storer R4, R7</t>
   </si>
   <si>
@@ -190,6 +151,51 @@
   </si>
   <si>
     <t>45 if test passes, 0 if test fails</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>setn R6, 0</t>
+  </si>
+  <si>
+    <t>jeqzn R6, 14</t>
+  </si>
+  <si>
+    <t>jeqzn R1, 30</t>
+  </si>
+  <si>
+    <t>jeqzn R2, 30</t>
+  </si>
+  <si>
+    <t>jnezn R1, 18</t>
+  </si>
+  <si>
+    <t>jnezn R2, 20</t>
+  </si>
+  <si>
+    <t>jnezn R2, 30</t>
+  </si>
+  <si>
+    <t>jgtzn R1, 23</t>
+  </si>
+  <si>
+    <t>jgtzn R2, 30</t>
+  </si>
+  <si>
+    <t>jgtzn R6, 30</t>
+  </si>
+  <si>
+    <t>jltzn R2, 27</t>
+  </si>
+  <si>
+    <t>jltzn R1, 30</t>
+  </si>
+  <si>
+    <t>jltzn R6, 30</t>
+  </si>
+  <si>
+    <t>jumpn 31</t>
   </si>
 </sst>
 </file>
@@ -261,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -270,6 +276,24 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -586,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543BF97D-9911-42E4-8549-403F59348339}">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -599,7 +623,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -653,31 +677,31 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C4">
         <v>40</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
+      <c r="D4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
@@ -693,23 +717,23 @@
       <c r="D5">
         <v>5</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
+      <c r="E5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="M5" t="s">
         <v>12</v>
@@ -729,28 +753,28 @@
       <c r="D6">
         <v>5</v>
       </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
+      <c r="E6" s="7">
+        <v>5</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
-        <f t="shared" ref="A7:A35" si="0">A6+1</f>
+        <f t="shared" ref="A7:A36" si="0">A6+1</f>
         <v>3</v>
       </c>
       <c r="B7" t="s">
@@ -762,23 +786,23 @@
       <c r="D7">
         <v>5</v>
       </c>
-      <c r="E7">
-        <v>-5</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
+      <c r="E7" s="7">
+        <v>-5</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
@@ -795,24 +819,24 @@
       <c r="D8">
         <v>5</v>
       </c>
-      <c r="E8">
-        <v>-5</v>
-      </c>
-      <c r="F8">
+      <c r="E8" s="7">
+        <v>-5</v>
+      </c>
+      <c r="F8" s="7">
         <f>C8+E8</f>
         <v>35</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
+      <c r="G8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
@@ -829,25 +853,25 @@
       <c r="D9">
         <v>5</v>
       </c>
-      <c r="E9">
-        <v>-5</v>
-      </c>
-      <c r="F9">
-        <f t="shared" ref="F9:F35" si="1">C9+E9</f>
-        <v>35</v>
-      </c>
-      <c r="G9">
+      <c r="E9" s="7">
+        <v>-5</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" ref="F9:F36" si="1">C9+E9</f>
+        <v>35</v>
+      </c>
+      <c r="G9" s="7">
         <f>C9-E9</f>
         <v>45</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
+      <c r="H9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
@@ -864,25 +888,25 @@
       <c r="D10" s="1">
         <v>5</v>
       </c>
-      <c r="E10" s="1">
-        <v>-5</v>
-      </c>
-      <c r="F10" s="1">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="G10" s="1">
+      <c r="E10" s="8">
+        <v>-5</v>
+      </c>
+      <c r="F10" s="8">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="G10" s="8">
         <f>C10-E10</f>
         <v>45</v>
       </c>
-      <c r="H10" s="1">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0</v>
+      <c r="H10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="L10" t="s">
         <v>27</v>
@@ -902,24 +926,24 @@
       <c r="D11" s="1">
         <v>5</v>
       </c>
-      <c r="E11" s="1">
-        <v>-5</v>
-      </c>
-      <c r="F11" s="1">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0</v>
+      <c r="E11" s="8">
+        <v>-5</v>
+      </c>
+      <c r="F11" s="8">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="L11" t="s">
         <v>24</v>
@@ -939,24 +963,24 @@
       <c r="D12" s="2">
         <v>5</v>
       </c>
-      <c r="E12" s="2">
-        <v>-5</v>
-      </c>
-      <c r="F12" s="2">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="G12" s="2">
-        <v>45</v>
-      </c>
-      <c r="H12" s="2">
-        <v>11</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0</v>
+      <c r="E12" s="9">
+        <v>-5</v>
+      </c>
+      <c r="F12" s="9">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="G12" s="9">
+        <v>45</v>
+      </c>
+      <c r="H12" s="9">
+        <v>11</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
@@ -973,24 +997,24 @@
       <c r="D13" s="2">
         <v>5</v>
       </c>
-      <c r="E13" s="2">
-        <v>-5</v>
-      </c>
-      <c r="F13" s="2">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="G13" s="2">
-        <v>45</v>
-      </c>
-      <c r="H13" s="2">
-        <v>11</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0</v>
+      <c r="E13" s="9">
+        <v>-5</v>
+      </c>
+      <c r="F13" s="9">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="G13" s="9">
+        <v>45</v>
+      </c>
+      <c r="H13" s="9">
+        <v>11</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="L13" t="s">
         <v>27</v>
@@ -1010,33 +1034,32 @@
       <c r="D14" s="2">
         <v>5</v>
       </c>
-      <c r="E14" s="2">
-        <v>-5</v>
-      </c>
-      <c r="F14" s="2">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0</v>
-      </c>
-      <c r="H14" s="2">
-        <v>11</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0</v>
+      <c r="E14" s="9">
+        <v>-5</v>
+      </c>
+      <c r="F14" s="9">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="G14" s="9">
+        <v>0</v>
+      </c>
+      <c r="H14" s="9">
+        <v>11</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
-        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C15" s="3">
         <v>40</v>
@@ -1060,20 +1083,16 @@
       <c r="I15" s="3">
         <v>0</v>
       </c>
-      <c r="J15" s="3">
-        <v>0</v>
-      </c>
-      <c r="L15" t="s">
-        <v>18</v>
+      <c r="J15" s="10" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
-        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C16" s="3">
         <v>40</v>
@@ -1089,7 +1108,7 @@
         <v>35</v>
       </c>
       <c r="G16" s="3">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="H16" s="3">
         <v>11</v>
@@ -1097,8 +1116,11 @@
       <c r="I16" s="3">
         <v>0</v>
       </c>
-      <c r="J16" s="3">
-        <v>0</v>
+      <c r="J16" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L16" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
@@ -1107,7 +1129,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C17" s="3">
         <v>40</v>
@@ -1123,7 +1145,7 @@
         <v>35</v>
       </c>
       <c r="G17" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="H17" s="3">
         <v>11</v>
@@ -1131,11 +1153,8 @@
       <c r="I17" s="3">
         <v>0</v>
       </c>
-      <c r="J17" s="3">
-        <v>0</v>
-      </c>
-      <c r="L17" t="s">
-        <v>17</v>
+      <c r="J17" s="10" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
@@ -1144,7 +1163,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C18" s="3">
         <v>40</v>
@@ -1168,48 +1187,48 @@
       <c r="I18" s="3">
         <v>0</v>
       </c>
-      <c r="J18" s="3">
-        <v>0</v>
+      <c r="J18" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="L18" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="4">
-        <v>40</v>
-      </c>
-      <c r="D19" s="4">
-        <v>5</v>
-      </c>
-      <c r="E19" s="4">
-        <v>-5</v>
-      </c>
-      <c r="F19" s="4">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="G19" s="4">
-        <v>45</v>
-      </c>
-      <c r="H19" s="4">
-        <v>11</v>
-      </c>
-      <c r="I19" s="4">
-        <v>0</v>
-      </c>
-      <c r="J19" s="4">
-        <v>0</v>
+      <c r="B19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="3">
+        <v>40</v>
+      </c>
+      <c r="D19" s="3">
+        <v>5</v>
+      </c>
+      <c r="E19" s="3">
+        <v>-5</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="G19" s="3">
+        <v>45</v>
+      </c>
+      <c r="H19" s="3">
+        <v>11</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="L19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
@@ -1218,7 +1237,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C20" s="4">
         <v>40</v>
@@ -1234,7 +1253,7 @@
         <v>35</v>
       </c>
       <c r="G20" s="4">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="H20" s="4">
         <v>11</v>
@@ -1242,8 +1261,11 @@
       <c r="I20" s="4">
         <v>0</v>
       </c>
-      <c r="J20" s="4">
-        <v>0</v>
+      <c r="J20" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L20" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
@@ -1252,7 +1274,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C21" s="4">
         <v>40</v>
@@ -1268,7 +1290,7 @@
         <v>35</v>
       </c>
       <c r="G21" s="4">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="H21" s="4">
         <v>11</v>
@@ -1276,11 +1298,8 @@
       <c r="I21" s="4">
         <v>0</v>
       </c>
-      <c r="J21" s="4">
-        <v>0</v>
-      </c>
-      <c r="L21" t="s">
-        <v>18</v>
+      <c r="J21" s="11" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
@@ -1289,7 +1308,7 @@
         <v>18</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="C22" s="4">
         <v>40</v>
@@ -1305,7 +1324,7 @@
         <v>35</v>
       </c>
       <c r="G22" s="4">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="H22" s="4">
         <v>11</v>
@@ -1313,8 +1332,11 @@
       <c r="I22" s="4">
         <v>0</v>
       </c>
-      <c r="J22" s="4">
-        <v>0</v>
+      <c r="J22" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L22" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
@@ -1323,7 +1345,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C23" s="4">
         <v>40</v>
@@ -1339,7 +1361,7 @@
         <v>35</v>
       </c>
       <c r="G23" s="4">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="H23" s="4">
         <v>11</v>
@@ -1347,48 +1369,45 @@
       <c r="I23" s="4">
         <v>0</v>
       </c>
-      <c r="J23" s="4">
-        <v>0</v>
-      </c>
-      <c r="L23" t="s">
+      <c r="J23" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="4">
+        <v>40</v>
+      </c>
+      <c r="D24" s="4">
+        <v>5</v>
+      </c>
+      <c r="E24" s="4">
+        <v>-5</v>
+      </c>
+      <c r="F24" s="4">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="G24" s="4">
+        <v>45</v>
+      </c>
+      <c r="H24" s="4">
+        <v>11</v>
+      </c>
+      <c r="I24" s="4">
+        <v>0</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L24" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A24" s="5">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="5">
-        <v>40</v>
-      </c>
-      <c r="D24" s="5">
-        <v>5</v>
-      </c>
-      <c r="E24" s="5">
-        <v>-5</v>
-      </c>
-      <c r="F24" s="5">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="G24" s="5">
-        <v>45</v>
-      </c>
-      <c r="H24" s="5">
-        <v>11</v>
-      </c>
-      <c r="I24" s="5">
-        <v>0</v>
-      </c>
-      <c r="J24" s="5">
-        <v>0</v>
-      </c>
-      <c r="L24" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
@@ -1397,7 +1416,7 @@
         <v>21</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C25" s="5">
         <v>40</v>
@@ -1413,7 +1432,7 @@
         <v>35</v>
       </c>
       <c r="G25" s="5">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="H25" s="5">
         <v>11</v>
@@ -1421,16 +1440,20 @@
       <c r="I25" s="5">
         <v>0</v>
       </c>
-      <c r="J25" s="5">
-        <v>0</v>
+      <c r="J25" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L25" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C26" s="5">
         <v>40</v>
@@ -1446,7 +1469,7 @@
         <v>35</v>
       </c>
       <c r="G26" s="5">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="H26" s="5">
         <v>11</v>
@@ -1454,11 +1477,8 @@
       <c r="I26" s="5">
         <v>0</v>
       </c>
-      <c r="J26" s="5">
-        <v>0</v>
-      </c>
-      <c r="L26" t="s">
-        <v>17</v>
+      <c r="J26" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
@@ -1466,7 +1486,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C27" s="5">
         <v>40</v>
@@ -1490,47 +1510,47 @@
       <c r="I27" s="5">
         <v>0</v>
       </c>
-      <c r="J27" s="5">
-        <v>0</v>
+      <c r="J27" s="12" t="s">
+        <v>40</v>
       </c>
       <c r="L27" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A28" s="6">
+      <c r="A28" s="5">
         <v>24</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="6">
-        <v>40</v>
-      </c>
-      <c r="D28" s="6">
-        <v>5</v>
-      </c>
-      <c r="E28" s="6">
-        <v>-5</v>
-      </c>
-      <c r="F28" s="6">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="G28" s="6">
-        <v>45</v>
-      </c>
-      <c r="H28" s="6">
-        <v>11</v>
-      </c>
-      <c r="I28" s="6">
-        <v>0</v>
-      </c>
-      <c r="J28" s="6">
-        <v>0</v>
+      <c r="B28" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="5">
+        <v>40</v>
+      </c>
+      <c r="D28" s="5">
+        <v>5</v>
+      </c>
+      <c r="E28" s="5">
+        <v>-5</v>
+      </c>
+      <c r="F28" s="5">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="G28" s="5">
+        <v>45</v>
+      </c>
+      <c r="H28" s="5">
+        <v>11</v>
+      </c>
+      <c r="I28" s="5">
+        <v>0</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>40</v>
       </c>
       <c r="L28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
@@ -1538,7 +1558,7 @@
         <v>25</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C29" s="6">
         <v>40</v>
@@ -1554,7 +1574,7 @@
         <v>35</v>
       </c>
       <c r="G29" s="6">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="H29" s="6">
         <v>11</v>
@@ -1562,8 +1582,11 @@
       <c r="I29" s="6">
         <v>0</v>
       </c>
-      <c r="J29" s="6">
-        <v>0</v>
+      <c r="J29" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="L29" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
@@ -1571,7 +1594,7 @@
         <v>26</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C30" s="6">
         <v>40</v>
@@ -1587,7 +1610,7 @@
         <v>35</v>
       </c>
       <c r="G30" s="6">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="H30" s="6">
         <v>11</v>
@@ -1595,11 +1618,8 @@
       <c r="I30" s="6">
         <v>0</v>
       </c>
-      <c r="J30" s="6">
-        <v>0</v>
-      </c>
-      <c r="L30" t="s">
-        <v>17</v>
+      <c r="J30" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.35">
@@ -1607,7 +1627,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C31" s="6">
         <v>40</v>
@@ -1631,45 +1651,47 @@
       <c r="I31" s="6">
         <v>0</v>
       </c>
-      <c r="J31" s="6">
-        <v>0</v>
+      <c r="J31" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="L31" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A32">
-        <f t="shared" si="0"/>
+      <c r="A32" s="6">
         <v>28</v>
       </c>
-      <c r="B32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32">
-        <v>40</v>
-      </c>
-      <c r="D32">
-        <v>5</v>
-      </c>
-      <c r="E32">
-        <v>-5</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="G32">
-        <v>45</v>
-      </c>
-      <c r="H32">
-        <v>11</v>
-      </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-      <c r="J32">
-        <v>0</v>
+      <c r="B32" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="6">
+        <v>40</v>
+      </c>
+      <c r="D32" s="6">
+        <v>5</v>
+      </c>
+      <c r="E32" s="6">
+        <v>-5</v>
+      </c>
+      <c r="F32" s="6">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="G32" s="6">
+        <v>45</v>
+      </c>
+      <c r="H32" s="6">
+        <v>11</v>
+      </c>
+      <c r="I32" s="6">
+        <v>0</v>
+      </c>
+      <c r="J32" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="L32" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
@@ -1678,7 +1700,7 @@
         <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="C33">
         <v>40</v>
@@ -1702,11 +1724,8 @@
       <c r="I33">
         <v>0</v>
       </c>
-      <c r="J33">
-        <v>0</v>
-      </c>
-      <c r="L33" t="s">
-        <v>25</v>
+      <c r="J33" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
@@ -1715,7 +1734,7 @@
         <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C34">
         <v>40</v>
@@ -1739,8 +1758,11 @@
       <c r="I34">
         <v>0</v>
       </c>
-      <c r="J34">
-        <v>41</v>
+      <c r="J34" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L34" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
@@ -1749,7 +1771,7 @@
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C35">
         <v>40</v>
@@ -1776,43 +1798,77 @@
       <c r="J35">
         <v>41</v>
       </c>
-      <c r="M35" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>44</v>
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36">
+        <v>40</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+      <c r="E36">
+        <v>-5</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="G36">
+        <v>45</v>
+      </c>
+      <c r="H36">
+        <v>11</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>41</v>
+      </c>
+      <c r="M36" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38">
-        <v>40</v>
-      </c>
-      <c r="B38">
-        <v>5</v>
-      </c>
-      <c r="L38" t="s">
-        <v>47</v>
+      <c r="A38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39">
+        <v>40</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="L39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A40">
         <v>41</v>
       </c>
-      <c r="B39" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="L39" t="s">
-        <v>52</v>
+      <c r="B40" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L40" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>